<commit_message>
Modified the xpath and updated the excel files
</commit_message>
<xml_diff>
--- a/target/test-classes/Excel/NaukriData.xlsx
+++ b/target/test-classes/Excel/NaukriData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\Downloads\eclipse-jee-2024-06-R-win32-x86_64\eclipse\eclipse-workspace\JavaJ2EE\NaukriProject\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4ED3A0-2182-4D39-9E24-167A3C914CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A8E230-AB52-4F5F-93C3-554BAC020462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1464" yWindow="1464" windowWidth="19176" windowHeight="9996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -586,7 +586,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="6">
-        <v>80</v>
+        <v>3.5</v>
       </c>
       <c r="M2" t="s">
         <v>21</v>

</xml_diff>